<commit_message>
ADD extra fields and change titles to noncaps in course list XLSX file
</commit_message>
<xml_diff>
--- a/CourseList.xlsx
+++ b/CourseList.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smitty\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F5DE383-DF74-482B-AD6C-67D9B169821D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFA2EB10-E248-4697-93DC-078C5356CB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14610" xr2:uid="{4039291D-6A13-4452-B4A5-9AE0E1DDD2AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Course" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,31 +37,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>COURSE NAME</t>
-  </si>
-  <si>
-    <t>COURSE ID</t>
-  </si>
-  <si>
-    <t>COURSE LINK</t>
-  </si>
-  <si>
-    <t>COURSE AUTHOR</t>
-  </si>
-  <si>
-    <t>CERTIFICATE</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Microsof Excel 2016 Master Class: Beginner to Advanced</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/excel-2016-tutorial</t>
+  </si>
+  <si>
+    <t>Bruce Myron</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Date Started</t>
+  </si>
+  <si>
+    <t>Date Finished</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>CourseID</t>
+  </si>
+  <si>
+    <t>Course Name</t>
+  </si>
+  <si>
+    <t>Course Link</t>
+  </si>
+  <si>
+    <t>Course Author</t>
+  </si>
+  <si>
+    <t>Certificate</t>
+  </si>
+  <si>
+    <t>Lesson</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Section</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,13 +119,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -400,39 +442,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{792224ED-F7C7-4F7E-8E27-99721D590B93}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="F2" s="2">
+        <v>45147</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2">
+        <v>45148</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{AE1F0D64-FD85-47CD-9323-8AD5DB8E3B13}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05342721-E8C1-487D-A3DC-B94B85771E4D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6DFAE98-206C-4390-8F53-7FB252C5CA4B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add TJ Walker Freelance course to course list XLSX file
</commit_message>
<xml_diff>
--- a/CourseList.xlsx
+++ b/CourseList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smitty\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFA2EB10-E248-4697-93DC-078C5356CB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F522EA-4943-4930-ABBB-9B97DF291887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14610" xr2:uid="{4039291D-6A13-4452-B4A5-9AE0E1DDD2AE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Microsof Excel 2016 Master Class: Beginner to Advanced</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Section</t>
+  </si>
+  <si>
+    <t>The Guide To Freelancing in the Modern Gig Economy</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/how-to-be-a-successful-freelancer-in-the-modern-gig-economy</t>
+  </si>
+  <si>
+    <t>TJ Walker</t>
   </si>
 </sst>
 </file>
@@ -442,17 +451,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{792224ED-F7C7-4F7E-8E27-99721D590B93}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="90.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
@@ -523,12 +532,42 @@
         <v>45148</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45056</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>12</v>
+      </c>
+      <c r="J3" s="2">
+        <v>45056</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{AE1F0D64-FD85-47CD-9323-8AD5DB8E3B13}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{D1D40196-14BD-433E-A9A7-09581779EC22}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
MOD current lesson on course list XLSX file
</commit_message>
<xml_diff>
--- a/CourseList.xlsx
+++ b/CourseList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smitty\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F522EA-4943-4930-ABBB-9B97DF291887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECB5EBE-D9F9-400A-9A28-07C329BEBAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14610" xr2:uid="{4039291D-6A13-4452-B4A5-9AE0E1DDD2AE}"/>
   </bookViews>
@@ -555,7 +555,7 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="J3" s="2">
         <v>45056</v>

</xml_diff>

<commit_message>
ADD 365 Careers financial anaylst course to course list XLSX file
</commit_message>
<xml_diff>
--- a/CourseList.xlsx
+++ b/CourseList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smitty\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECB5EBE-D9F9-400A-9A28-07C329BEBAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9A2AA9-6958-408F-8537-E72330342326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14610" xr2:uid="{4039291D-6A13-4452-B4A5-9AE0E1DDD2AE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Microsof Excel 2016 Master Class: Beginner to Advanced</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>TJ Walker</t>
+  </si>
+  <si>
+    <t>The Complete Financial Analyst Course 2023</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/the-complete-financial-analyst-course</t>
+  </si>
+  <si>
+    <t>365 Careers</t>
   </si>
 </sst>
 </file>
@@ -451,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{792224ED-F7C7-4F7E-8E27-99721D590B93}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,13 +570,37 @@
         <v>45056</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45057</v>
+      </c>
+      <c r="J4" s="2">
+        <v>45057</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{AE1F0D64-FD85-47CD-9323-8AD5DB8E3B13}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{D1D40196-14BD-433E-A9A7-09581779EC22}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{DE6A4D9C-D845-4F96-BE80-6075EBF0D77B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
UPDATE sections and lessons in course list XLSX file
</commit_message>
<xml_diff>
--- a/CourseList.xlsx
+++ b/CourseList.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smitty\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9A2AA9-6958-408F-8537-E72330342326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE1D122-1F7F-49EC-8FF4-0C224B0E097A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14610" xr2:uid="{4039291D-6A13-4452-B4A5-9AE0E1DDD2AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Course" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Author" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Microsof Excel 2016 Master Class: Beginner to Advanced</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>365 Careers</t>
+  </si>
+  <si>
+    <t>AuthorID</t>
+  </si>
+  <si>
+    <t>Author Name</t>
   </si>
 </sst>
 </file>
@@ -463,7 +469,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,13 +538,13 @@
         <v>45147</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I2">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="J2" s="2">
-        <v>45148</v>
+        <v>45058</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -561,13 +567,13 @@
         <v>45056</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I3">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="J3" s="2">
-        <v>45056</v>
+        <v>45058</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -588,6 +594,12 @@
       </c>
       <c r="F4" s="2">
         <v>45057</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>9</v>
       </c>
       <c r="J4" s="2">
         <v>45057</v>
@@ -606,12 +618,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05342721-E8C1-487D-A3DC-B94B85771E4D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
FIX months in date fileds and ADD drupal from basics to advance with 3 live projects course to course list XLSX file
</commit_message>
<xml_diff>
--- a/CourseList.xlsx
+++ b/CourseList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smitty\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE1D122-1F7F-49EC-8FF4-0C224B0E097A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0281041-E037-4E73-8EAA-69F58B6A27E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14610" xr2:uid="{4039291D-6A13-4452-B4A5-9AE0E1DDD2AE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Microsof Excel 2016 Master Class: Beginner to Advanced</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>Author Name</t>
+  </si>
+  <si>
+    <t>Drupal From Basics to Advance with 3 Live Projects</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/advanced-web-development-with-drupal</t>
+  </si>
+  <si>
+    <t>Abdul Rehman</t>
   </si>
 </sst>
 </file>
@@ -466,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{792224ED-F7C7-4F7E-8E27-99721D590B93}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +553,7 @@
         <v>21</v>
       </c>
       <c r="J2" s="2">
-        <v>45058</v>
+        <v>45150</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -564,7 +573,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="2">
-        <v>45056</v>
+        <v>45148</v>
       </c>
       <c r="H3">
         <v>4</v>
@@ -573,7 +582,7 @@
         <v>42</v>
       </c>
       <c r="J3" s="2">
-        <v>45058</v>
+        <v>45150</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -593,7 +602,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="2">
-        <v>45057</v>
+        <v>45149</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -602,7 +611,36 @@
         <v>9</v>
       </c>
       <c r="J4" s="2">
-        <v>45057</v>
+        <v>45149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45150</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2">
+        <v>45150</v>
       </c>
     </row>
   </sheetData>
@@ -610,9 +648,10 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{AE1F0D64-FD85-47CD-9323-8AD5DB8E3B13}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{D1D40196-14BD-433E-A9A7-09581779EC22}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{DE6A4D9C-D845-4F96-BE80-6075EBF0D77B}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{3BA9FB36-330E-442D-A325-C3BE5B36111E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>